<commit_message>
Notebooks v10 without detailed soils
</commit_message>
<xml_diff>
--- a/Analysis/Data/DetailedSoils.xlsx
+++ b/Analysis/Data/DetailedSoils.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8960" yWindow="1100" windowWidth="27760" windowHeight="16240" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="8960" yWindow="1100" windowWidth="27760" windowHeight="16240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Conc-D3" sheetId="1" r:id="rId1"/>
@@ -1184,7 +1184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -2601,10 +2601,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13:G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F66" sqref="F66:F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2636,7 +2637,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>119</v>
       </c>
@@ -2660,7 +2661,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>120</v>
       </c>
@@ -2684,7 +2685,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -2708,7 +2709,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>122</v>
       </c>
@@ -2736,7 +2737,7 @@
         <v>0.79086471662352054</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>123</v>
       </c>
@@ -2760,7 +2761,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -2784,7 +2785,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>122</v>
       </c>
@@ -2808,7 +2809,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>123</v>
       </c>
@@ -2832,7 +2833,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>125</v>
       </c>
@@ -2856,7 +2857,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>126</v>
       </c>
@@ -2880,7 +2881,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>127</v>
       </c>
@@ -2904,7 +2905,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>128</v>
       </c>
@@ -2928,7 +2929,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>129</v>
       </c>
@@ -2952,7 +2953,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>130</v>
       </c>
@@ -2979,7 +2980,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>73</v>
       </c>
@@ -3010,7 +3011,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -3045,7 +3046,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>75</v>
       </c>
@@ -3076,7 +3077,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -3107,7 +3108,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -3138,7 +3139,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -3169,7 +3170,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -3204,7 +3205,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>80</v>
       </c>
@@ -3229,7 +3230,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -3260,7 +3261,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>82</v>
       </c>
@@ -3285,7 +3286,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>83</v>
       </c>
@@ -3316,7 +3317,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>84</v>
       </c>
@@ -3347,7 +3348,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>85</v>
       </c>
@@ -3378,7 +3379,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -3409,7 +3410,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -3440,7 +3441,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -3471,7 +3472,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -3497,7 +3498,7 @@
       </c>
       <c r="K32" s="11"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -3523,7 +3524,7 @@
       </c>
       <c r="K33" s="11"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>91</v>
       </c>
@@ -3548,7 +3549,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>92</v>
       </c>
@@ -3573,7 +3574,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>93</v>
       </c>
@@ -3598,7 +3599,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>94</v>
       </c>
@@ -3623,7 +3624,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>95</v>
       </c>
@@ -3648,7 +3649,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>96</v>
       </c>
@@ -3673,7 +3674,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -3698,7 +3699,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -3723,7 +3724,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>99</v>
       </c>
@@ -3748,7 +3749,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>100</v>
       </c>
@@ -3777,7 +3778,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>101</v>
       </c>
@@ -3802,7 +3803,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>102</v>
       </c>
@@ -3827,7 +3828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>103</v>
       </c>
@@ -3852,7 +3853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>104</v>
       </c>
@@ -3877,7 +3878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>105</v>
       </c>
@@ -3902,7 +3903,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>106</v>
       </c>
@@ -3927,7 +3928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>107</v>
       </c>
@@ -3952,7 +3953,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>108</v>
       </c>
@@ -3977,7 +3978,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>109</v>
       </c>
@@ -4002,7 +4003,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>110</v>
       </c>
@@ -4027,7 +4028,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>111</v>
       </c>
@@ -4052,7 +4053,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>112</v>
       </c>
@@ -4077,7 +4078,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>113</v>
       </c>
@@ -4102,7 +4103,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>114</v>
       </c>
@@ -4127,7 +4128,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>115</v>
       </c>
@@ -4152,7 +4153,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>116</v>
       </c>
@@ -4177,7 +4178,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>117</v>
       </c>
@@ -4202,7 +4203,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>118</v>
       </c>
@@ -4227,7 +4228,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>131</v>
       </c>
@@ -4252,7 +4253,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>132</v>
       </c>
@@ -4277,7 +4278,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>133</v>
       </c>
@@ -4302,7 +4303,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>134</v>
       </c>
@@ -4402,7 +4403,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>138</v>
       </c>
@@ -4427,7 +4428,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>139</v>
       </c>
@@ -4452,7 +4453,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>140</v>
       </c>
@@ -4477,7 +4478,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>141</v>
       </c>
@@ -4502,7 +4503,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>142</v>
       </c>
@@ -4527,7 +4528,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>143</v>
       </c>
@@ -4552,7 +4553,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>144</v>
       </c>
@@ -4577,7 +4578,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>145</v>
       </c>
@@ -4602,7 +4603,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>146</v>
       </c>
@@ -4627,7 +4628,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>147</v>
       </c>
@@ -4652,7 +4653,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>148</v>
       </c>
@@ -4677,7 +4678,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>149</v>
       </c>
@@ -4702,7 +4703,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>150</v>
       </c>
@@ -4727,7 +4728,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>151</v>
       </c>
@@ -4752,7 +4753,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>152</v>
       </c>
@@ -4777,7 +4778,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>150</v>
       </c>
@@ -4802,7 +4803,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>151</v>
       </c>
@@ -4827,7 +4828,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>151</v>
       </c>
@@ -4852,7 +4853,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>151</v>
       </c>
@@ -4877,7 +4878,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>152</v>
       </c>
@@ -4902,7 +4903,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>153</v>
       </c>
@@ -4931,7 +4932,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>154</v>
       </c>
@@ -4956,7 +4957,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>155</v>
       </c>
@@ -4981,7 +4982,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>156</v>
       </c>
@@ -5006,7 +5007,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>157</v>
       </c>
@@ -5031,7 +5032,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>158</v>
       </c>
@@ -5056,7 +5057,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>159</v>
       </c>
@@ -5081,7 +5082,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>160</v>
       </c>
@@ -5106,7 +5107,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>161</v>
       </c>
@@ -5135,7 +5136,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>162</v>
       </c>
@@ -5160,7 +5161,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>163</v>
       </c>
@@ -5185,7 +5186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>164</v>
       </c>
@@ -5210,7 +5211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>165</v>
       </c>
@@ -5235,7 +5236,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>166</v>
       </c>
@@ -5260,7 +5261,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>167</v>
       </c>
@@ -5285,7 +5286,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>168</v>
       </c>
@@ -5310,7 +5311,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>169</v>
       </c>
@@ -5335,7 +5336,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>170</v>
       </c>
@@ -5360,7 +5361,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>171</v>
       </c>
@@ -5385,7 +5386,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>172</v>
       </c>
@@ -5410,7 +5411,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>173</v>
       </c>
@@ -5435,7 +5436,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>174</v>
       </c>
@@ -5464,7 +5465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>175</v>
       </c>
@@ -5489,7 +5490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>176</v>
       </c>
@@ -5514,7 +5515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>177</v>
       </c>
@@ -5539,7 +5540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>178</v>
       </c>
@@ -5568,7 +5569,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>179</v>
       </c>
@@ -5593,7 +5594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>180</v>
       </c>
@@ -5618,7 +5619,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>181</v>
       </c>
@@ -5643,7 +5644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>182</v>
       </c>
@@ -5668,7 +5669,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>183</v>
       </c>
@@ -5693,7 +5694,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>184</v>
       </c>
@@ -5718,7 +5719,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>185</v>
       </c>
@@ -5743,7 +5744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>186</v>
       </c>
@@ -5768,7 +5769,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>187</v>
       </c>
@@ -5797,7 +5798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>188</v>
       </c>
@@ -5822,7 +5823,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>189</v>
       </c>
@@ -5847,7 +5848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>190</v>
       </c>
@@ -5872,7 +5873,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>191</v>
       </c>
@@ -5897,7 +5898,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>192</v>
       </c>
@@ -5922,7 +5923,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>193</v>
       </c>
@@ -5947,7 +5948,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>194</v>
       </c>
@@ -5976,7 +5977,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>195</v>
       </c>
@@ -6001,7 +6002,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>188</v>
       </c>
@@ -6026,7 +6027,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>187</v>
       </c>
@@ -6051,7 +6052,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>196</v>
       </c>
@@ -6080,7 +6081,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>197</v>
       </c>
@@ -6105,7 +6106,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>198</v>
       </c>
@@ -6130,7 +6131,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>199</v>
       </c>
@@ -6155,7 +6156,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>200</v>
       </c>
@@ -6184,7 +6185,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>192</v>
       </c>
@@ -6209,7 +6210,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>201</v>
       </c>
@@ -6234,7 +6235,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>193</v>
       </c>
@@ -6259,7 +6260,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>194</v>
       </c>
@@ -6284,7 +6285,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>202</v>
       </c>
@@ -6309,7 +6310,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>195</v>
       </c>
@@ -6334,7 +6335,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>188</v>
       </c>
@@ -6359,7 +6360,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>187</v>
       </c>
@@ -6384,7 +6385,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>197</v>
       </c>
@@ -6409,7 +6410,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>198</v>
       </c>
@@ -6434,7 +6435,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>199</v>
       </c>
@@ -6460,7 +6461,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K149"/>
+  <autoFilter ref="A1:K149">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="S-III-13"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed bug in getTestOutput() function
</commit_message>
<xml_diff>
--- a/Analysis/Data/DetailedSoils.xlsx
+++ b/Analysis/Data/DetailedSoils.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DayTightChunks/Documents/PhD/Models/.nosync/pesti-beach16/Analysis/Data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8960" yWindow="1100" windowWidth="27760" windowHeight="16240" tabRatio="500"/>
+    <workbookView xWindow="8955" yWindow="1095" windowWidth="27765" windowHeight="16245" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Conc-D3" sheetId="1" r:id="rId1"/>
@@ -20,11 +15,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Conc-D3'!$A$1:$H$59</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Isotopes-D3'!$A$1:$K$149</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -875,38 +867,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="33">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1174,7 +1166,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1184,13 +1176,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1216,7 +1208,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1240,7 +1232,7 @@
         <v>42458</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1264,7 +1256,7 @@
         <v>42458</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1288,7 +1280,7 @@
         <v>42458</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1312,7 +1304,7 @@
         <v>42458</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1336,7 +1328,7 @@
         <v>42458</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1360,7 +1352,7 @@
         <v>42458</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1384,7 +1376,7 @@
         <v>42458</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1408,7 +1400,7 @@
         <v>42507</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1432,7 +1424,7 @@
         <v>42474</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1456,7 +1448,7 @@
         <v>42507</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1480,7 +1472,7 @@
         <v>42474</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1504,7 +1496,7 @@
         <v>42474</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1528,7 +1520,7 @@
         <v>42502</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1547,7 +1539,7 @@
       </c>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1568,7 +1560,7 @@
         <v>42521</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1587,7 +1579,7 @@
       </c>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1611,7 +1603,7 @@
         <v>42521</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1635,7 +1627,7 @@
         <v>42521</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1659,7 +1651,7 @@
         <v>42563</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1683,7 +1675,7 @@
         <v>42549</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1707,7 +1699,7 @@
         <v>42563</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1731,7 +1723,7 @@
         <v>42563</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1755,7 +1747,7 @@
         <v>42563</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1776,7 +1768,7 @@
         <v>42563</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1800,7 +1792,7 @@
         <v>42563</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1824,7 +1816,7 @@
         <v>42458</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1848,7 +1840,7 @@
         <v>42458</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1872,7 +1864,7 @@
         <v>42458</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1896,7 +1888,7 @@
         <v>42458</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1920,7 +1912,7 @@
         <v>42458</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1944,7 +1936,7 @@
         <v>42458</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1968,7 +1960,7 @@
         <v>42474</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1992,7 +1984,7 @@
         <v>42507</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2016,7 +2008,7 @@
         <v>42474</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2040,7 +2032,7 @@
         <v>42474</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -2064,7 +2056,7 @@
         <v>42542</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -2088,7 +2080,7 @@
         <v>42542</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -2112,7 +2104,7 @@
         <v>42521</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2136,7 +2128,7 @@
         <v>42535</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2160,7 +2152,7 @@
         <v>42521</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2184,7 +2176,7 @@
         <v>42521</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -2208,7 +2200,7 @@
         <v>42502</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -2232,7 +2224,7 @@
         <v>42563</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -2256,7 +2248,7 @@
         <v>42563</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2280,7 +2272,7 @@
         <v>42563</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2304,7 +2296,7 @@
         <v>42563</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -2328,7 +2320,7 @@
         <v>42549</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -2352,7 +2344,7 @@
         <v>42563</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -2376,7 +2368,7 @@
         <v>42459</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -2400,7 +2392,7 @@
         <v>42459</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -2424,7 +2416,7 @@
         <v>42459</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -2448,7 +2440,7 @@
         <v>42474</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2472,7 +2464,7 @@
         <v>42502</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2496,7 +2488,7 @@
         <v>42521</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -2520,7 +2512,7 @@
         <v>42521</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -2544,7 +2536,7 @@
         <v>42549</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -2568,7 +2560,7 @@
         <v>42563</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -2601,20 +2593,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K149"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F66" sqref="F66:F68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" customWidth="1"/>
+    <col min="10" max="10" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -2637,7 +2628,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>119</v>
       </c>
@@ -2661,7 +2652,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>120</v>
       </c>
@@ -2685,7 +2676,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -2709,7 +2700,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>122</v>
       </c>
@@ -2737,7 +2728,7 @@
         <v>0.79086471662352054</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>123</v>
       </c>
@@ -2761,7 +2752,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -2785,7 +2776,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>122</v>
       </c>
@@ -2809,7 +2800,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>123</v>
       </c>
@@ -2833,7 +2824,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>125</v>
       </c>
@@ -2857,7 +2848,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>126</v>
       </c>
@@ -2881,7 +2872,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>127</v>
       </c>
@@ -2905,7 +2896,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>128</v>
       </c>
@@ -2929,7 +2920,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>129</v>
       </c>
@@ -2953,7 +2944,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>130</v>
       </c>
@@ -2980,7 +2971,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>73</v>
       </c>
@@ -2998,7 +2989,7 @@
         <f>IF(H16=35,1,IF(H16=34,2,IF(H16=33,3,IF(H16=42,4,IF(H16=23,5,IF(H16=22,7,IF(H16=21,8,IF(H16=40,11,IF(H16=25,10,IF(H16=45,9,H16))))))))))</f>
         <v>2</v>
       </c>
-      <c r="G16" s="13">
+      <c r="F16" s="13">
         <v>-33.868000000000002</v>
       </c>
       <c r="H16" s="13">
@@ -3011,7 +3002,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -3033,8 +3024,8 @@
         <v>-30.552</v>
       </c>
       <c r="G17">
-        <f>STDEVA(F17,F18,F35,F36)</f>
-        <v>0.11357339770679804</v>
+        <f>STDEVA(F34,F17,F18,F35,F36,F16)</f>
+        <v>1.3592525029098426</v>
       </c>
       <c r="H17">
         <v>2</v>
@@ -3046,7 +3037,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>75</v>
       </c>
@@ -3077,7 +3068,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -3108,7 +3099,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -3139,7 +3130,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -3170,7 +3161,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -3205,7 +3196,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>80</v>
       </c>
@@ -3230,7 +3221,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -3261,7 +3252,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>82</v>
       </c>
@@ -3286,7 +3277,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>83</v>
       </c>
@@ -3317,7 +3308,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>84</v>
       </c>
@@ -3348,7 +3339,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>85</v>
       </c>
@@ -3379,7 +3370,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -3410,7 +3401,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -3441,7 +3432,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -3459,7 +3450,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>-30.753999999999998</v>
       </c>
       <c r="H31">
@@ -3472,7 +3463,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -3490,7 +3481,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>-31.276</v>
       </c>
       <c r="H32">
@@ -3498,7 +3489,7 @@
       </c>
       <c r="K32" s="11"/>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -3516,7 +3507,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>-31.673999999999999</v>
       </c>
       <c r="H33">
@@ -3524,7 +3515,7 @@
       </c>
       <c r="K33" s="11"/>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>91</v>
       </c>
@@ -3542,14 +3533,14 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G34">
+      <c r="F34">
         <v>-32.392000000000003</v>
       </c>
       <c r="H34">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>92</v>
       </c>
@@ -3574,7 +3565,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>93</v>
       </c>
@@ -3599,7 +3590,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>94</v>
       </c>
@@ -3624,7 +3615,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>95</v>
       </c>
@@ -3649,7 +3640,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>96</v>
       </c>
@@ -3674,7 +3665,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -3692,14 +3683,14 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>-31.684999999999999</v>
       </c>
       <c r="H40">
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -3717,14 +3708,14 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>-31.58</v>
       </c>
       <c r="H41">
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>99</v>
       </c>
@@ -3742,14 +3733,14 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>-30.893000000000001</v>
       </c>
       <c r="H42">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>100</v>
       </c>
@@ -3767,18 +3758,14 @@
         <f>IF(H43=35,1,IF(H43=34,2,IF(H43=33,3,IF(H43=42,4,IF(H43=23,5,IF(H43=22,7,IF(H43=21,8,IF(H43=40,11,IF(H43=25,10,IF(H43=45,9,H43))))))))))</f>
         <v>3</v>
       </c>
-      <c r="F43">
+      <c r="G43">
         <v>-26.995999999999999</v>
-      </c>
-      <c r="G43">
-        <f>STDEVA(F43,F44)</f>
-        <v>0.45820519420888256</v>
       </c>
       <c r="H43">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>101</v>
       </c>
@@ -3796,14 +3783,14 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>-27.643999999999998</v>
       </c>
       <c r="H44">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>102</v>
       </c>
@@ -3828,7 +3815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>103</v>
       </c>
@@ -3853,7 +3840,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>104</v>
       </c>
@@ -3878,7 +3865,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>105</v>
       </c>
@@ -3903,7 +3890,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>106</v>
       </c>
@@ -3921,14 +3908,14 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="F49">
+      <c r="G49">
         <v>-28.56</v>
       </c>
       <c r="H49">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>107</v>
       </c>
@@ -3946,14 +3933,14 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="F50">
+      <c r="G50">
         <v>-29.062999999999999</v>
       </c>
       <c r="H50">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>108</v>
       </c>
@@ -3971,14 +3958,14 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="F51">
+      <c r="G51">
         <v>-29.067999999999998</v>
       </c>
       <c r="H51">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>109</v>
       </c>
@@ -4003,7 +3990,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>110</v>
       </c>
@@ -4028,7 +4015,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>111</v>
       </c>
@@ -4053,7 +4040,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>112</v>
       </c>
@@ -4078,7 +4065,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>113</v>
       </c>
@@ -4103,7 +4090,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>114</v>
       </c>
@@ -4128,7 +4115,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>115</v>
       </c>
@@ -4153,7 +4140,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>116</v>
       </c>
@@ -4178,7 +4165,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>117</v>
       </c>
@@ -4203,7 +4190,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>118</v>
       </c>
@@ -4228,7 +4215,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>131</v>
       </c>
@@ -4253,7 +4240,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>132</v>
       </c>
@@ -4278,7 +4265,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>133</v>
       </c>
@@ -4303,7 +4290,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>134</v>
       </c>
@@ -4328,7 +4315,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>135</v>
       </c>
@@ -4353,7 +4340,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>136</v>
       </c>
@@ -4378,7 +4365,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>137</v>
       </c>
@@ -4403,7 +4390,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>138</v>
       </c>
@@ -4428,7 +4415,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>139</v>
       </c>
@@ -4453,7 +4440,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>140</v>
       </c>
@@ -4478,7 +4465,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>141</v>
       </c>
@@ -4503,7 +4490,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>142</v>
       </c>
@@ -4528,7 +4515,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>143</v>
       </c>
@@ -4553,7 +4540,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>144</v>
       </c>
@@ -4571,14 +4558,14 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="F75">
+      <c r="G75">
         <v>-30.667999999999999</v>
       </c>
       <c r="H75">
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>145</v>
       </c>
@@ -4596,14 +4583,14 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="F76">
+      <c r="G76">
         <v>-31.349999999999998</v>
       </c>
       <c r="H76">
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>146</v>
       </c>
@@ -4621,14 +4608,14 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="F77">
+      <c r="G77">
         <v>-30.332999999999998</v>
       </c>
       <c r="H77">
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>147</v>
       </c>
@@ -4653,7 +4640,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>148</v>
       </c>
@@ -4678,7 +4665,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>149</v>
       </c>
@@ -4703,7 +4690,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>150</v>
       </c>
@@ -4728,7 +4715,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>151</v>
       </c>
@@ -4753,7 +4740,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>152</v>
       </c>
@@ -4778,7 +4765,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>150</v>
       </c>
@@ -4803,7 +4790,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>151</v>
       </c>
@@ -4828,7 +4815,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>151</v>
       </c>
@@ -4853,7 +4840,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>151</v>
       </c>
@@ -4878,7 +4865,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>152</v>
       </c>
@@ -4903,7 +4890,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>153</v>
       </c>
@@ -4932,7 +4919,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>154</v>
       </c>
@@ -4957,7 +4944,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>155</v>
       </c>
@@ -4982,7 +4969,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>156</v>
       </c>
@@ -5007,7 +4994,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>157</v>
       </c>
@@ -5032,7 +5019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>158</v>
       </c>
@@ -5057,7 +5044,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>159</v>
       </c>
@@ -5082,7 +5069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>160</v>
       </c>
@@ -5107,7 +5094,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>161</v>
       </c>
@@ -5136,7 +5123,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>162</v>
       </c>
@@ -5161,7 +5148,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>163</v>
       </c>
@@ -5186,7 +5173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>164</v>
       </c>
@@ -5211,7 +5198,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>165</v>
       </c>
@@ -5229,14 +5216,14 @@
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="F101">
+      <c r="G101">
         <v>-29.654</v>
       </c>
       <c r="H101">
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>166</v>
       </c>
@@ -5254,14 +5241,14 @@
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="F102">
+      <c r="G102">
         <v>-26.983000000000001</v>
       </c>
       <c r="H102">
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>167</v>
       </c>
@@ -5279,14 +5266,14 @@
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="F103">
+      <c r="G103">
         <v>-29.425999999999998</v>
       </c>
       <c r="H103">
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>168</v>
       </c>
@@ -5311,7 +5298,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>169</v>
       </c>
@@ -5336,7 +5323,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>170</v>
       </c>
@@ -5361,7 +5348,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>171</v>
       </c>
@@ -5386,7 +5373,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>172</v>
       </c>
@@ -5411,7 +5398,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>173</v>
       </c>
@@ -5436,7 +5423,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>174</v>
       </c>
@@ -5465,7 +5452,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>175</v>
       </c>
@@ -5490,7 +5477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>176</v>
       </c>
@@ -5515,7 +5502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>177</v>
       </c>
@@ -5540,7 +5527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>178</v>
       </c>
@@ -5569,7 +5556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>179</v>
       </c>
@@ -5594,7 +5581,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>180</v>
       </c>
@@ -5619,7 +5606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>181</v>
       </c>
@@ -5644,7 +5631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>182</v>
       </c>
@@ -5669,7 +5656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>183</v>
       </c>
@@ -5694,7 +5681,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>184</v>
       </c>
@@ -5719,7 +5706,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>185</v>
       </c>
@@ -5744,7 +5731,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>186</v>
       </c>
@@ -5769,7 +5756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>187</v>
       </c>
@@ -5798,7 +5785,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>188</v>
       </c>
@@ -5823,7 +5810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>189</v>
       </c>
@@ -5848,7 +5835,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>190</v>
       </c>
@@ -5873,7 +5860,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>191</v>
       </c>
@@ -5898,7 +5885,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>192</v>
       </c>
@@ -5923,7 +5910,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>193</v>
       </c>
@@ -5948,12 +5935,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>194</v>
       </c>
       <c r="B130" t="str">
-        <f t="shared" ref="B130:B161" si="10">CONCATENATE(C130,"-",D130,"-",E130)</f>
+        <f t="shared" ref="B130:B149" si="10">CONCATENATE(C130,"-",D130,"-",E130)</f>
         <v>S-IV-12</v>
       </c>
       <c r="C130" t="s">
@@ -5977,7 +5964,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>195</v>
       </c>
@@ -6002,7 +5989,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>188</v>
       </c>
@@ -6027,7 +6014,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>187</v>
       </c>
@@ -6052,7 +6039,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>196</v>
       </c>
@@ -6081,7 +6068,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>197</v>
       </c>
@@ -6106,7 +6093,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>198</v>
       </c>
@@ -6131,7 +6118,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>199</v>
       </c>
@@ -6156,7 +6143,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>200</v>
       </c>
@@ -6185,7 +6172,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>192</v>
       </c>
@@ -6210,7 +6197,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>201</v>
       </c>
@@ -6235,7 +6222,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>193</v>
       </c>
@@ -6260,7 +6247,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>194</v>
       </c>
@@ -6285,7 +6272,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>202</v>
       </c>
@@ -6310,7 +6297,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>195</v>
       </c>
@@ -6335,7 +6322,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>188</v>
       </c>
@@ -6360,7 +6347,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>187</v>
       </c>
@@ -6385,7 +6372,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>197</v>
       </c>
@@ -6410,7 +6397,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>198</v>
       </c>
@@ -6435,7 +6422,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>199</v>
       </c>
@@ -6461,13 +6448,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K149">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="S-III-13"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K149"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -6481,9 +6462,9 @@
       <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>205</v>
       </c>
@@ -6491,7 +6472,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>207</v>
       </c>
@@ -6499,7 +6480,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>209</v>
       </c>
@@ -6507,7 +6488,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>211</v>
       </c>
@@ -6515,7 +6496,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>213</v>
       </c>
@@ -6523,7 +6504,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>215</v>
       </c>
@@ -6531,7 +6512,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>217</v>
       </c>

</xml_diff>